<commit_message>
- Serilog : log to file  - Code review for better error handling  - ERROR_CODES: unhandled exception
</commit_message>
<xml_diff>
--- a/PUBLIC.API/_ERROR_CODES.xlsx
+++ b/PUBLIC.API/_ERROR_CODES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoits\source\repos\SAAS.PUBLIC\PUBLIC.API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B279B28F-76B2-4500-BAB3-9E7BE87BB6DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF88290E-A1EC-4437-9243-4C7CFB1D9922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48FEAE66-0D95-43C3-9BB7-68A36BE352AF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
   <si>
     <t>Code</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>File fingerprint check failed for file 'dsfsdfsdF.pdf'</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>PUBLIC_API_99999</t>
+  </si>
+  <si>
+    <t>Unhandled exceptions</t>
   </si>
 </sst>
 </file>
@@ -303,8 +312,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D7B1F89-CEBA-4048-BC49-F8597046EE4B}" name="Table2" displayName="Table2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E29" xr:uid="{198720AF-A94A-4B71-BBB8-D904A4A640AE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D7B1F89-CEBA-4048-BC49-F8597046EE4B}" name="Table2" displayName="Table2" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E31" xr:uid="{198720AF-A94A-4B71-BBB8-D904A4A640AE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DEF6E48B-A865-44DB-AA6D-12D9B5140362}" name="Controller" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{44846A0D-25B1-41BB-A6AA-A4493EBCBB77}" name="Function" dataDxfId="3"/>
@@ -613,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA8AC2A-061C-42A7-AA6D-360B87A2453A}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,6 +1045,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>